<commit_message>
telnet端口失败 Signed-off-by: componey_qss <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/问题与解答.xlsx
+++ b/问题与解答.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21240" windowHeight="12165" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="js" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="tp32" sheetId="3" r:id="rId3"/>
     <sheet name="git" sheetId="4" r:id="rId4"/>
     <sheet name="composer" sheetId="5" r:id="rId5"/>
+    <sheet name="linux" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -113,8 +114,40 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Administrator</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Administrator:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ajax加载数据不多，request sent time却很长。后台没有任何处理，直接返回。依旧请求很长时间。ajax加载大数据。大文件。</t>
   </si>
@@ -131,7 +164,7 @@
     <t>centos7</t>
   </si>
   <si>
-    <t>composer install updateing卡了半天，结果gile could not be downloaded</t>
+    <t>composer install。 updateing卡了半天，结果gile could not be downloaded</t>
   </si>
   <si>
     <t>解决</t>
@@ -142,16 +175,19 @@
   <si>
     <t>https://blog.csdn.net/jqjtqq/article/details/80377924</t>
   </si>
+  <si>
+    <t>端口telnet失败</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -178,6 +214,113 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -199,113 +342,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -333,6 +369,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -363,126 +543,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -490,30 +550,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,26 +563,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,6 +589,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,17 +637,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,145 +668,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1419,7 +1455,7 @@
   <dimension ref="C2:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1447,4 +1483,30 @@
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="D3:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="3" spans="4:5">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
调整整体架构 Signed-off-by: fengjinliang <fengjinliang@streamhub.tech>
</commit_message>
<xml_diff>
--- a/问题与解答.xlsx
+++ b/问题与解答.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11670"/>
+    <workbookView windowWidth="14415" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>关键词</t>
   </si>
@@ -182,6 +182,9 @@
     <t>Yii:$app-&gt;request[console|web]先web的</t>
   </si>
   <si>
+    <t>yii2的异常处理？response？site/index?</t>
+  </si>
+  <si>
     <t>认证  协议</t>
   </si>
   <si>
@@ -215,6 +218,24 @@
     <t>php manual首页，各种扩展。安装及其作用</t>
   </si>
   <si>
+    <t>nginx的配置</t>
+  </si>
+  <si>
+    <t>php-fpm的配置</t>
+  </si>
+  <si>
+    <t>php.ini的配置</t>
+  </si>
+  <si>
+    <t>沙箱</t>
+  </si>
+  <si>
+    <t>mysql ---  mariadb</t>
+  </si>
+  <si>
+    <t>nginx --- tengine  淘宝web服务器</t>
+  </si>
+  <si>
     <t>ajax加载数据不多，request sent time却很长。后台没有任何处理，直接返回。依旧请求很长时间。ajax加载大数据。大文件。</t>
   </si>
   <si>
@@ -261,6 +282,9 @@
   </si>
   <si>
     <t>a用户再A分支上写的代码。现在想提交再B分支上？？可以吗</t>
+  </si>
+  <si>
+    <t>gui如何查看具体某个文件(如index.php)的历史</t>
   </si>
   <si>
     <r>
@@ -830,6 +854,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -838,8 +899,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -853,6 +945,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -862,118 +992,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF444444"/>
       <name val="Consolas"/>
@@ -1006,13 +1030,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,7 +1150,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1036,157 +1204,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1215,6 +1239,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1224,17 +1263,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1264,40 +1297,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1312,6 +1321,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1320,10 +1344,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1332,133 +1356,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1844,10 +1868,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D1:I32"/>
+  <dimension ref="D1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1928,15 +1952,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="15" spans="7:7">
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="17" customFormat="1" spans="4:7">
       <c r="D17" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>20191119</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="4:7">
@@ -1945,7 +1974,7 @@
         <v>20191119</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="4:7">
@@ -1954,7 +1983,7 @@
         <v>20191119</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="1" spans="4:7">
@@ -1963,18 +1992,18 @@
         <v>20191120</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="4:7">
       <c r="D25" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25">
         <v>20191120</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="5:7">
@@ -1982,7 +2011,7 @@
         <v>20191129</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="4:7">
@@ -1992,7 +2021,7 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="4:7">
@@ -2008,7 +2037,7 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" customFormat="1" spans="4:7">
@@ -2017,7 +2046,52 @@
         <v>20191128</v>
       </c>
       <c r="G32" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7">
+      <c r="E35">
+        <v>20191202</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7">
+      <c r="E36">
+        <v>20191202</v>
+      </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7">
+      <c r="E37">
+        <v>20191202</v>
+      </c>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7">
+      <c r="E39">
+        <v>20191218</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7">
+      <c r="E42">
+        <v>20191223</v>
+      </c>
+      <c r="G42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7">
+      <c r="G43" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2054,10 +2128,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -2254,7 +2328,7 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2269,8 +2343,8 @@
   <sheetPr/>
   <dimension ref="C2:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2281,151 +2355,156 @@
   <sheetData>
     <row r="2" spans="3:4">
       <c r="C2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>37</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="11:11">
       <c r="K28" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="11:11">
       <c r="K29" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="11:11">
       <c r="K30" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="11:11">
       <c r="K31" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="11:11">
       <c r="K33" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="11:11">
       <c r="K34" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" ht="26.25" spans="11:11">
       <c r="K36" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="11:11">
       <c r="K37" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="11:11">
       <c r="K38" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" ht="14.25"/>
     <row r="42" ht="24.75" spans="11:11">
       <c r="K42" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="11:11">
       <c r="K44" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="11:11">
       <c r="K47" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="11:11">
       <c r="K48" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="11:11">
       <c r="K49" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="11:11">
       <c r="K50" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="11:11">
       <c r="K51" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="11:11">
       <c r="K52" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2452,16 +2531,16 @@
   <sheetData>
     <row r="2" ht="31" customHeight="1" spans="3:6">
       <c r="C2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2484,10 +2563,10 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
php扩展/php-static/php-reflection Signed-off-by: fengjinliang <fengjinliang@streamhub.tech>
</commit_message>
<xml_diff>
--- a/问题与解答.xlsx
+++ b/问题与解答.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14415" windowHeight="12195"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="学习计划" sheetId="7" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t>关键词</t>
   </si>
@@ -236,6 +236,15 @@
     <t>nginx --- tengine  淘宝web服务器</t>
   </si>
   <si>
+    <t>mysql 外键 优劣</t>
+  </si>
+  <si>
+    <t>mysql中【两位小数】decial(8,2)还是string?</t>
+  </si>
+  <si>
+    <t>mysql中的引擎innob和myisam是对数据库的还是对表的？</t>
+  </si>
+  <si>
     <t>ajax加载数据不多，request sent time却很长。后台没有任何处理，直接返回。依旧请求很长时间。ajax加载大数据。大文件。</t>
   </si>
   <si>
@@ -285,6 +294,9 @@
   </si>
   <si>
     <t>gui如何查看具体某个文件(如index.php)的历史</t>
+  </si>
+  <si>
+    <t>用小乌龟工具</t>
   </si>
   <si>
     <r>
@@ -803,8 +815,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="30">
@@ -855,9 +867,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -869,23 +904,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -899,11 +949,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -914,9 +963,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,8 +986,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,59 +1010,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF444444"/>
       <name val="Consolas"/>
@@ -1030,43 +1042,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,97 +1204,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,37 +1222,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,7 +1270,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1267,7 +1279,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1297,16 +1324,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1321,21 +1348,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1344,10 +1356,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1356,133 +1368,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1868,10 +1880,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D1:I43"/>
+  <dimension ref="D1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2092,6 +2104,24 @@
     <row r="43" spans="7:7">
       <c r="G43" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7">
+      <c r="E46">
+        <v>20200103</v>
+      </c>
+      <c r="G46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7">
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7">
+      <c r="G48" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2128,10 +2158,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -2328,7 +2358,7 @@
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2344,7 +2374,7 @@
   <dimension ref="C2:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2355,156 +2385,159 @@
   <sheetData>
     <row r="2" spans="3:4">
       <c r="C2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="3:3">
       <c r="C9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="3:3">
       <c r="C11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
       <c r="C23" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="11:11">
       <c r="K28" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="11:11">
       <c r="K29" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="11:11">
       <c r="K30" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="11:11">
       <c r="K31" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="11:11">
       <c r="K33" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="11:11">
       <c r="K34" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" ht="26.25" spans="11:11">
       <c r="K36" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="11:11">
       <c r="K37" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="11:11">
       <c r="K38" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" ht="14.25"/>
     <row r="42" ht="24.75" spans="11:11">
       <c r="K42" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="11:11">
       <c r="K44" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="11:11">
       <c r="K47" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="11:11">
       <c r="K48" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="11:11">
       <c r="K49" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="11:11">
       <c r="K50" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="11:11">
       <c r="K51" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="11:11">
       <c r="K52" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2531,16 +2564,16 @@
   <sheetData>
     <row r="2" ht="31" customHeight="1" spans="3:6">
       <c r="C2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2563,10 +2596,10 @@
   <sheetData>
     <row r="3" spans="4:5">
       <c r="D3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>